<commit_message>
added foreign key + check
</commit_message>
<xml_diff>
--- a/lib.xlsx
+++ b/lib.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hojun\Desktop\UVA\6th sem\CS 4750\FootballDatabase\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="339">
   <si>
     <t>No</t>
   </si>
@@ -1025,17 +1030,25 @@
   </si>
   <si>
     <t>CA</t>
+  </si>
+  <si>
+    <t>Team</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lib</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1043,8 +1056,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1056,7 +1076,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1079,13 +1099,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1094,6 +1128,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1140,7 +1182,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1172,9 +1214,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1206,6 +1266,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1381,14 +1459,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I92"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J92" sqref="A2:J92"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1413,8 +1493,11 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1442,8 +1525,11 @@
       <c r="I2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1471,8 +1557,11 @@
       <c r="I3" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1500,8 +1589,11 @@
       <c r="I4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1529,8 +1621,11 @@
       <c r="I5" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1558,8 +1653,11 @@
       <c r="I6" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1587,8 +1685,11 @@
       <c r="I7" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1616,8 +1717,11 @@
       <c r="I8" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1645,8 +1749,11 @@
       <c r="I9" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1674,8 +1781,11 @@
       <c r="I10" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1703,8 +1813,11 @@
       <c r="I11" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1732,8 +1845,11 @@
       <c r="I12" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1761,8 +1877,11 @@
       <c r="I13" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1790,8 +1909,11 @@
       <c r="I14" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1819,8 +1941,11 @@
       <c r="I15" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1848,8 +1973,11 @@
       <c r="I16" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1877,8 +2005,11 @@
       <c r="I17" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1906,8 +2037,11 @@
       <c r="I18" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1935,8 +2069,11 @@
       <c r="I19" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1964,8 +2101,11 @@
       <c r="I20" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1993,8 +2133,11 @@
       <c r="I21" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2022,8 +2165,11 @@
       <c r="I22" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2051,8 +2197,11 @@
       <c r="I23" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2080,8 +2229,11 @@
       <c r="I24" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2109,8 +2261,11 @@
       <c r="I25" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2138,8 +2293,11 @@
       <c r="I26" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2167,8 +2325,11 @@
       <c r="I27" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2196,8 +2357,11 @@
       <c r="I28" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2225,8 +2389,11 @@
       <c r="I29" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2254,8 +2421,11 @@
       <c r="I30" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2283,8 +2453,11 @@
       <c r="I31" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2312,8 +2485,11 @@
       <c r="I32" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="J32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2341,8 +2517,11 @@
       <c r="I33" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2370,8 +2549,11 @@
       <c r="I34" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2399,8 +2581,11 @@
       <c r="I35" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2428,8 +2613,11 @@
       <c r="I36" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="J36" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2457,8 +2645,11 @@
       <c r="I37" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="J37" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2486,8 +2677,11 @@
       <c r="I38" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="J38" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2515,8 +2709,11 @@
       <c r="I39" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="J39" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2544,8 +2741,11 @@
       <c r="I40" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="J40" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2573,8 +2773,11 @@
       <c r="I41" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="J41" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2602,8 +2805,11 @@
       <c r="I42" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="J42" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2631,8 +2837,11 @@
       <c r="I43" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="J43" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2660,8 +2869,11 @@
       <c r="I44" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="J44" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2689,8 +2901,11 @@
       <c r="I45" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="J45" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2718,8 +2933,11 @@
       <c r="I46" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2747,8 +2965,11 @@
       <c r="I47" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="J47" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2776,8 +2997,11 @@
       <c r="I48" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="J48" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2805,8 +3029,11 @@
       <c r="I49" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="J49" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2834,8 +3061,11 @@
       <c r="I50" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2863,8 +3093,11 @@
       <c r="I51" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="J51" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2892,8 +3125,11 @@
       <c r="I52" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="J52" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2921,8 +3157,11 @@
       <c r="I53" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="J53" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2950,8 +3189,11 @@
       <c r="I54" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="J54" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2979,8 +3221,11 @@
       <c r="I55" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="J55" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3008,8 +3253,11 @@
       <c r="I56" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="J56" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3037,8 +3285,11 @@
       <c r="I57" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="J57" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3066,8 +3317,11 @@
       <c r="I58" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="J58" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3095,8 +3349,11 @@
       <c r="I59" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="J59" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3124,8 +3381,11 @@
       <c r="I60" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="J60" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3153,8 +3413,11 @@
       <c r="I61" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="J61" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3182,8 +3445,11 @@
       <c r="I62" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="J62" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -3211,8 +3477,11 @@
       <c r="I63" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="J63" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -3240,8 +3509,11 @@
       <c r="I64" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="J64" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -3269,8 +3541,11 @@
       <c r="I65" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="66" spans="1:9">
+      <c r="J65" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -3298,8 +3573,11 @@
       <c r="I66" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="67" spans="1:9">
+      <c r="J66" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -3327,8 +3605,11 @@
       <c r="I67" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="J67" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -3356,8 +3637,11 @@
       <c r="I68" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="69" spans="1:9">
+      <c r="J68" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -3385,8 +3669,11 @@
       <c r="I69" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="70" spans="1:9">
+      <c r="J69" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -3414,8 +3701,11 @@
       <c r="I70" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="71" spans="1:9">
+      <c r="J70" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -3443,8 +3733,11 @@
       <c r="I71" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="72" spans="1:9">
+      <c r="J71" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -3472,8 +3765,11 @@
       <c r="I72" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="73" spans="1:9">
+      <c r="J72" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -3501,8 +3797,11 @@
       <c r="I73" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="74" spans="1:9">
+      <c r="J73" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -3530,8 +3829,11 @@
       <c r="I74" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="75" spans="1:9">
+      <c r="J74" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -3559,8 +3861,11 @@
       <c r="I75" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="76" spans="1:9">
+      <c r="J75" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -3588,8 +3893,11 @@
       <c r="I76" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="77" spans="1:9">
+      <c r="J76" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -3617,8 +3925,11 @@
       <c r="I77" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="J77" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -3646,8 +3957,11 @@
       <c r="I78" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="J78" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -3675,8 +3989,11 @@
       <c r="I79" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="J79" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -3704,8 +4021,11 @@
       <c r="I80" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="J80" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -3733,8 +4053,11 @@
       <c r="I81" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="J81" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -3762,8 +4085,11 @@
       <c r="I82" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="J82" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -3791,8 +4117,11 @@
       <c r="I83" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="J83" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3820,8 +4149,11 @@
       <c r="I84" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="J84" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3849,8 +4181,11 @@
       <c r="I85" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="J85" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3878,8 +4213,11 @@
       <c r="I86" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="J86" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3907,8 +4245,11 @@
       <c r="I87" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="J87" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3936,8 +4277,11 @@
       <c r="I88" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="J88" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3965,8 +4309,11 @@
       <c r="I89" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="90" spans="1:9">
+      <c r="J89" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3994,8 +4341,11 @@
       <c r="I90" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="J90" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -4023,8 +4373,11 @@
       <c r="I91" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="92" spans="1:9">
+      <c r="J91" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -4052,8 +4405,12 @@
       <c r="I92" t="s">
         <v>253</v>
       </c>
+      <c r="J92" t="s">
+        <v>338</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated foriegn key with cascade + exported all db sql file.
</commit_message>
<xml_diff>
--- a/lib.xlsx
+++ b/lib.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="340">
   <si>
     <t>No</t>
   </si>
@@ -1037,6 +1037,10 @@
   </si>
   <si>
     <t>Lib</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1460,15 +1464,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:K92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J92" sqref="A2:J92"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1496,8 +1500,11 @@
       <c r="J1" s="2" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K1" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1528,8 +1535,11 @@
       <c r="J2" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K2">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1560,8 +1570,11 @@
       <c r="J3" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K3">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1592,8 +1605,11 @@
       <c r="J4" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K4">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1624,8 +1640,11 @@
       <c r="J5" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K5">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1656,8 +1675,11 @@
       <c r="J6" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K6">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1688,8 +1710,11 @@
       <c r="J7" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K7">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1720,8 +1745,11 @@
       <c r="J8" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K8">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1752,8 +1780,11 @@
       <c r="J9" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K9">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1784,8 +1815,11 @@
       <c r="J10" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K10">
+        <v>3009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1816,8 +1850,11 @@
       <c r="J11" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K11">
+        <v>3010</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1848,8 +1885,11 @@
       <c r="J12" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K12">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1880,8 +1920,11 @@
       <c r="J13" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K13">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1912,8 +1955,11 @@
       <c r="J14" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K14">
+        <v>3013</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1944,8 +1990,11 @@
       <c r="J15" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K15">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1976,8 +2025,11 @@
       <c r="J16" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K16">
+        <v>3015</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2008,8 +2060,11 @@
       <c r="J17" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K17">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2040,8 +2095,11 @@
       <c r="J18" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K18">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2072,8 +2130,11 @@
       <c r="J19" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K19">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2104,8 +2165,11 @@
       <c r="J20" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K20">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2136,8 +2200,11 @@
       <c r="J21" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K21">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2168,8 +2235,11 @@
       <c r="J22" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K22">
+        <v>3021</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2200,8 +2270,11 @@
       <c r="J23" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K23">
+        <v>3022</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2232,8 +2305,11 @@
       <c r="J24" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K24">
+        <v>3023</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2264,8 +2340,11 @@
       <c r="J25" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K25">
+        <v>3024</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2296,8 +2375,11 @@
       <c r="J26" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K26">
+        <v>3025</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2328,8 +2410,11 @@
       <c r="J27" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K27">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2360,8 +2445,11 @@
       <c r="J28" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K28">
+        <v>3027</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2392,8 +2480,11 @@
       <c r="J29" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K29">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2424,8 +2515,11 @@
       <c r="J30" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K30">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2456,8 +2550,11 @@
       <c r="J31" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K31">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2488,8 +2585,11 @@
       <c r="J32" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K32">
+        <v>3031</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2520,8 +2620,11 @@
       <c r="J33" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K33">
+        <v>3032</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2552,8 +2655,11 @@
       <c r="J34" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K34">
+        <v>3033</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2584,8 +2690,11 @@
       <c r="J35" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K35">
+        <v>3034</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2616,8 +2725,11 @@
       <c r="J36" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K36">
+        <v>3035</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2648,8 +2760,11 @@
       <c r="J37" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K37">
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2680,8 +2795,11 @@
       <c r="J38" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K38">
+        <v>3037</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2712,8 +2830,11 @@
       <c r="J39" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K39">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2744,8 +2865,11 @@
       <c r="J40" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K40">
+        <v>3039</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2776,8 +2900,11 @@
       <c r="J41" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K41">
+        <v>3040</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2808,8 +2935,11 @@
       <c r="J42" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K42">
+        <v>3041</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2840,8 +2970,11 @@
       <c r="J43" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K43">
+        <v>3042</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2872,8 +3005,11 @@
       <c r="J44" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K44">
+        <v>3043</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2904,8 +3040,11 @@
       <c r="J45" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K45">
+        <v>3044</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2936,8 +3075,11 @@
       <c r="J46" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K46">
+        <v>3045</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2968,8 +3110,11 @@
       <c r="J47" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K47">
+        <v>3046</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3000,8 +3145,11 @@
       <c r="J48" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K48">
+        <v>3047</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3032,8 +3180,11 @@
       <c r="J49" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K49">
+        <v>3048</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3064,8 +3215,11 @@
       <c r="J50" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K50">
+        <v>3049</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3096,8 +3250,11 @@
       <c r="J51" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K51">
+        <v>3050</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3128,8 +3285,11 @@
       <c r="J52" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K52">
+        <v>3051</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3160,8 +3320,11 @@
       <c r="J53" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K53">
+        <v>3052</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3192,8 +3355,11 @@
       <c r="J54" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K54">
+        <v>3053</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3224,8 +3390,11 @@
       <c r="J55" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K55">
+        <v>3054</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3256,8 +3425,11 @@
       <c r="J56" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K56">
+        <v>3055</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3288,8 +3460,11 @@
       <c r="J57" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K57">
+        <v>3056</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3320,8 +3495,11 @@
       <c r="J58" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K58">
+        <v>3057</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3352,8 +3530,11 @@
       <c r="J59" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K59">
+        <v>3058</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3384,8 +3565,11 @@
       <c r="J60" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K60">
+        <v>3059</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3416,8 +3600,11 @@
       <c r="J61" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K61">
+        <v>3060</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3448,8 +3635,11 @@
       <c r="J62" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K62">
+        <v>3061</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -3480,8 +3670,11 @@
       <c r="J63" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K63">
+        <v>3062</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -3512,8 +3705,11 @@
       <c r="J64" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K64">
+        <v>3063</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -3544,8 +3740,11 @@
       <c r="J65" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K65">
+        <v>3064</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -3576,8 +3775,11 @@
       <c r="J66" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K66">
+        <v>3065</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -3608,8 +3810,11 @@
       <c r="J67" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K67">
+        <v>3066</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -3640,8 +3845,11 @@
       <c r="J68" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K68">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -3672,8 +3880,11 @@
       <c r="J69" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K69">
+        <v>3068</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -3704,8 +3915,11 @@
       <c r="J70" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K70">
+        <v>3069</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -3736,8 +3950,11 @@
       <c r="J71" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K71">
+        <v>3070</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -3768,8 +3985,11 @@
       <c r="J72" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K72">
+        <v>3071</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -3800,8 +4020,11 @@
       <c r="J73" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K73">
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -3832,8 +4055,11 @@
       <c r="J74" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K74">
+        <v>3073</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -3864,8 +4090,11 @@
       <c r="J75" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K75">
+        <v>3074</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -3896,8 +4125,11 @@
       <c r="J76" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K76">
+        <v>3075</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -3928,8 +4160,11 @@
       <c r="J77" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K77">
+        <v>3076</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -3960,8 +4195,11 @@
       <c r="J78" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K78">
+        <v>3077</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -3992,8 +4230,11 @@
       <c r="J79" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K79">
+        <v>3078</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -4024,8 +4265,11 @@
       <c r="J80" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K80">
+        <v>3079</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -4056,8 +4300,11 @@
       <c r="J81" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K81">
+        <v>3080</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -4088,8 +4335,11 @@
       <c r="J82" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K82">
+        <v>3081</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -4120,8 +4370,11 @@
       <c r="J83" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K83">
+        <v>3082</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -4152,8 +4405,11 @@
       <c r="J84" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K84">
+        <v>3083</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -4184,8 +4440,11 @@
       <c r="J85" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K85">
+        <v>3084</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -4216,8 +4475,11 @@
       <c r="J86" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K86">
+        <v>3085</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -4248,8 +4510,11 @@
       <c r="J87" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K87">
+        <v>3086</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -4280,8 +4545,11 @@
       <c r="J88" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K88">
+        <v>3087</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -4312,8 +4580,11 @@
       <c r="J89" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K89">
+        <v>3088</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -4344,8 +4615,11 @@
       <c r="J90" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K90">
+        <v>3089</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -4376,8 +4650,11 @@
       <c r="J91" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K91">
+        <v>3090</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -4407,6 +4684,9 @@
       </c>
       <c r="J92" t="s">
         <v>338</v>
+      </c>
+      <c r="K92">
+        <v>3091</v>
       </c>
     </row>
   </sheetData>

</xml_diff>